<commit_message>
working on facings on displays kpi for pnghk-sand
</commit_message>
<xml_diff>
--- a/Projects/PNGHK_SAND/Data/PNGHK_template_2019_14_01.xlsx
+++ b/Projects/PNGHK_SAND/Data/PNGHK_template_2019_14_01.xlsx
@@ -12,10 +12,14 @@
     <sheet name="OSD_RULES" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$P$1:$P$85</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">OSD_RULES!$A$1:$H$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$P$1:$P$85</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">OSD_RULES!$A$1:$H$32</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">OSD_RULES!$A$1:$H$32</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">OSD_RULES!$A$1:$H$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">OSD_RULES!$A$1:$H$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">OSD_RULES!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1485,7 +1489,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1559,6 +1563,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1677,7 +1687,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1770,6 +1780,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1794,7 +1808,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1885,9 +1899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1897,7 +1911,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1927,9 +1941,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1939,7 +1953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1969,9 +1983,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1981,7 +1995,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2011,9 +2025,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2023,7 +2037,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2053,9 +2067,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2065,7 +2079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2095,9 +2109,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2107,7 +2121,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2137,9 +2151,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2149,7 +2163,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2179,9 +2193,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2191,7 +2205,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2221,9 +2235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2233,7 +2247,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2263,9 +2277,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2275,7 +2289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2305,9 +2319,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2317,7 +2331,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2347,9 +2361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2359,7 +2373,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2389,9 +2403,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2401,7 +2415,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2431,9 +2445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2443,7 +2457,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2473,9 +2487,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2485,7 +2499,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2515,9 +2529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2527,7 +2541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2557,9 +2571,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2569,7 +2583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2599,9 +2613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2611,7 +2625,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2641,9 +2655,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2653,7 +2667,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2683,9 +2697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2695,7 +2709,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2725,9 +2739,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2737,7 +2751,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2767,9 +2781,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2779,7 +2793,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2809,9 +2823,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2821,7 +2835,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2851,9 +2865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2863,7 +2877,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2893,9 +2907,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2905,7 +2919,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2935,9 +2949,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2947,7 +2961,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2977,9 +2991,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2989,7 +3003,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3019,9 +3033,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3031,7 +3045,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3061,9 +3075,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3073,7 +3087,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3103,9 +3117,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3115,7 +3129,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3145,9 +3159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3157,7 +3171,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3187,9 +3201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3199,7 +3213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3229,9 +3243,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3241,7 +3255,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3271,9 +3285,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3283,7 +3297,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3313,9 +3327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>716040</xdr:colOff>
+      <xdr:colOff>715320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3325,7 +3339,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6116400" cy="6352560"/>
+          <a:ext cx="5963400" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3355,9 +3369,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3367,7 +3381,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3400,9 +3414,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3412,7 +3426,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3445,9 +3459,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3457,7 +3471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3490,9 +3504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3502,7 +3516,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3535,9 +3549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3547,7 +3561,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3580,9 +3594,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3592,7 +3606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3625,9 +3639,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3637,7 +3651,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3670,9 +3684,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3682,7 +3696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3715,9 +3729,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3727,7 +3741,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3760,9 +3774,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3772,7 +3786,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3805,9 +3819,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3817,7 +3831,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3850,9 +3864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3862,7 +3876,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3895,9 +3909,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3907,7 +3921,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3940,9 +3954,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3952,7 +3966,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3985,9 +3999,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3997,7 +4011,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4030,9 +4044,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4042,7 +4056,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4075,9 +4089,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4087,7 +4101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4120,9 +4134,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4132,7 +4146,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4165,9 +4179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4177,7 +4191,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4210,9 +4224,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4222,7 +4236,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4255,9 +4269,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4267,7 +4281,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4300,9 +4314,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4312,7 +4326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4345,9 +4359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4357,7 +4371,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4390,9 +4404,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4402,7 +4416,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4435,9 +4449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4447,7 +4461,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4480,9 +4494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4492,7 +4506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4525,9 +4539,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4537,7 +4551,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4570,9 +4584,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4582,7 +4596,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4615,9 +4629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4627,7 +4641,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4660,9 +4674,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4672,7 +4686,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4705,9 +4719,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4717,7 +4731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4750,9 +4764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4762,7 +4776,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4795,9 +4809,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4807,7 +4821,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4840,9 +4854,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4852,7 +4866,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6186600" cy="6352920"/>
+          <a:ext cx="6033600" cy="6352200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4890,9 +4904,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>398880</xdr:colOff>
+      <xdr:colOff>398160</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4902,7 +4916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7304400" cy="11512800"/>
+          <a:ext cx="7132320" cy="11512080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4932,9 +4946,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>398880</xdr:colOff>
+      <xdr:colOff>398160</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4944,7 +4958,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7304400" cy="11512800"/>
+          <a:ext cx="7132320" cy="11512080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4974,9 +4988,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>398880</xdr:colOff>
+      <xdr:colOff>398160</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4986,7 +5000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7304400" cy="11512800"/>
+          <a:ext cx="7132320" cy="11512080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5016,9 +5030,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>398880</xdr:colOff>
+      <xdr:colOff>398160</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5028,7 +5042,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7304400" cy="11512800"/>
+          <a:ext cx="7132320" cy="11512080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5058,9 +5072,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>398880</xdr:colOff>
+      <xdr:colOff>398160</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5070,7 +5084,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7304400" cy="11512800"/>
+          <a:ext cx="7132320" cy="11512080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5100,9 +5114,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5112,7 +5126,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7412760" cy="6552360"/>
+          <a:ext cx="7240680" cy="6551640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5145,9 +5159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5157,7 +5171,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7412760" cy="6552360"/>
+          <a:ext cx="7240680" cy="6551640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5190,9 +5204,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5202,7 +5216,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7412760" cy="6552360"/>
+          <a:ext cx="7240680" cy="6551640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5235,9 +5249,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5247,7 +5261,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7412760" cy="6552360"/>
+          <a:ext cx="7240680" cy="6551640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5280,9 +5294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5292,7 +5306,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7412760" cy="6552360"/>
+          <a:ext cx="7240680" cy="6551640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5327,39 +5341,40 @@
   <dimension ref="A1:AJ85"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="L58" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
-      <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+      <selection pane="bottomRight" activeCell="P82" activeCellId="0" sqref="P82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="108.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="83.5612244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="20.25"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="97.0612244897959"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="58.8571428571429"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="60.4744897959184"/>
-    <col collapsed="false" hidden="false" max="36" min="24" style="5" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1021" min="37" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="105.831632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="81.6683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="94.765306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="57.5051020408163"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="58.9897959183674"/>
+    <col collapsed="false" hidden="false" max="36" min="24" style="5" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1021" min="37" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9526,8 +9541,8 @@
       <c r="M54" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N54" s="11" t="s">
-        <v>27</v>
+      <c r="N54" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O54" s="11" t="s">
         <v>27</v>
@@ -9604,8 +9619,8 @@
       <c r="M55" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N55" s="11" t="s">
-        <v>27</v>
+      <c r="N55" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O55" s="11" t="s">
         <v>27</v>
@@ -9756,8 +9771,8 @@
       <c r="M57" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N57" s="11" t="s">
-        <v>27</v>
+      <c r="N57" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O57" s="11" t="s">
         <v>27</v>
@@ -9834,8 +9849,8 @@
       <c r="M58" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N58" s="11" t="s">
-        <v>27</v>
+      <c r="N58" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O58" s="11" t="s">
         <v>27</v>
@@ -9910,7 +9925,7 @@
       <c r="M59" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N59" s="11" t="s">
+      <c r="N59" s="23" t="s">
         <v>26</v>
       </c>
       <c r="O59" s="11" t="s">
@@ -9986,8 +10001,8 @@
       <c r="M60" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N60" s="11" t="s">
-        <v>27</v>
+      <c r="N60" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O60" s="11" t="s">
         <v>27</v>
@@ -10064,8 +10079,8 @@
       <c r="M61" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N61" s="11" t="s">
-        <v>27</v>
+      <c r="N61" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O61" s="11" t="s">
         <v>27</v>
@@ -10120,7 +10135,7 @@
         <v>25</v>
       </c>
       <c r="E62" s="13"/>
-      <c r="F62" s="23"/>
+      <c r="F62" s="24"/>
       <c r="G62" s="21"/>
       <c r="H62" s="15" t="s">
         <v>26</v>
@@ -10218,8 +10233,8 @@
       <c r="M63" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N63" s="11" t="s">
-        <v>27</v>
+      <c r="N63" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O63" s="11" t="s">
         <v>27</v>
@@ -10298,8 +10313,8 @@
       <c r="M64" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N64" s="11" t="s">
-        <v>27</v>
+      <c r="N64" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O64" s="11" t="s">
         <v>27</v>
@@ -10376,7 +10391,7 @@
       <c r="M65" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N65" s="11" t="s">
+      <c r="N65" s="23" t="s">
         <v>26</v>
       </c>
       <c r="O65" s="11" t="s">
@@ -10454,8 +10469,8 @@
       <c r="M66" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N66" s="11" t="s">
-        <v>27</v>
+      <c r="N66" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O66" s="11" t="s">
         <v>27</v>
@@ -10534,8 +10549,8 @@
       <c r="M67" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N67" s="11" t="s">
-        <v>27</v>
+      <c r="N67" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O67" s="11" t="s">
         <v>27</v>
@@ -10690,8 +10705,8 @@
       <c r="M69" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N69" s="11" t="s">
-        <v>27</v>
+      <c r="N69" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O69" s="11" t="s">
         <v>27</v>
@@ -10770,8 +10785,8 @@
       <c r="M70" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N70" s="11" t="s">
-        <v>27</v>
+      <c r="N70" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O70" s="11" t="s">
         <v>27</v>
@@ -10848,7 +10863,7 @@
       <c r="M71" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N71" s="11" t="s">
+      <c r="N71" s="23" t="s">
         <v>26</v>
       </c>
       <c r="O71" s="11" t="s">
@@ -10926,8 +10941,8 @@
       <c r="M72" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N72" s="11" t="s">
-        <v>27</v>
+      <c r="N72" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O72" s="11" t="s">
         <v>27</v>
@@ -11006,8 +11021,8 @@
       <c r="M73" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N73" s="11" t="s">
-        <v>27</v>
+      <c r="N73" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O73" s="11" t="s">
         <v>27</v>
@@ -11162,8 +11177,8 @@
       <c r="M75" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N75" s="11" t="s">
-        <v>27</v>
+      <c r="N75" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O75" s="11" t="s">
         <v>27</v>
@@ -11242,8 +11257,8 @@
       <c r="M76" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N76" s="11" t="s">
-        <v>27</v>
+      <c r="N76" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O76" s="11" t="s">
         <v>27</v>
@@ -11398,8 +11413,8 @@
       <c r="M78" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N78" s="11" t="s">
-        <v>27</v>
+      <c r="N78" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O78" s="11" t="s">
         <v>27</v>
@@ -11478,8 +11493,8 @@
       <c r="M79" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N79" s="11" t="s">
-        <v>27</v>
+      <c r="N79" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="O79" s="11" t="s">
         <v>27</v>
@@ -11632,14 +11647,14 @@
       <c r="M81" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N81" s="11" t="s">
+      <c r="N81" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O81" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="P81" s="11" t="s">
-        <v>27</v>
+      <c r="P81" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="Q81" s="15" t="s">
         <v>40</v>
@@ -11676,7 +11691,7 @@
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="16"/>
-      <c r="G82" s="23"/>
+      <c r="G82" s="24"/>
       <c r="H82" s="15" t="s">
         <v>26</v>
       </c>
@@ -11695,7 +11710,7 @@
       <c r="M82" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N82" s="11" t="s">
+      <c r="N82" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O82" s="11" t="s">
@@ -11760,13 +11775,13 @@
       <c r="M83" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N83" s="11" t="s">
+      <c r="N83" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O83" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="P83" s="11" t="s">
+      <c r="P83" s="16" t="s">
         <v>26</v>
       </c>
       <c r="Q83" s="15" t="s">
@@ -11825,13 +11840,13 @@
       <c r="M84" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N84" s="11" t="s">
+      <c r="N84" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O84" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="P84" s="11" t="s">
+      <c r="P84" s="16" t="s">
         <v>26</v>
       </c>
       <c r="Q84" s="15" t="s">
@@ -11871,7 +11886,7 @@
         <v>95</v>
       </c>
       <c r="F85" s="16"/>
-      <c r="G85" s="24"/>
+      <c r="G85" s="25"/>
       <c r="H85" s="15" t="s">
         <v>26</v>
       </c>
@@ -11890,7 +11905,7 @@
       <c r="M85" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N85" s="11" t="s">
+      <c r="N85" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O85" s="11" t="s">
@@ -11920,6 +11935,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="P1:P85"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -11945,13 +11961,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11984,22 +12000,22 @@
       <c r="A2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="25" t="n">
+      <c r="F2" s="26" t="n">
         <v>7</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="28" t="s">
         <v>124</v>
       </c>
     </row>
@@ -12007,40 +12023,40 @@
       <c r="A3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="25" t="n">
+      <c r="F4" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="28" t="s">
         <v>124</v>
       </c>
     </row>
@@ -12048,40 +12064,40 @@
       <c r="A5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="25" t="n">
+      <c r="F6" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="28" t="s">
         <v>124</v>
       </c>
     </row>
@@ -12089,22 +12105,22 @@
       <c r="A7" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F7" s="25" t="n">
+      <c r="F7" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="28" t="s">
         <v>124</v>
       </c>
     </row>
@@ -12112,22 +12128,22 @@
       <c r="A8" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="25" t="n">
+      <c r="F8" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="28" t="s">
         <v>124</v>
       </c>
     </row>
@@ -12135,379 +12151,379 @@
       <c r="A9" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="L10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="L10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="L11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="L11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="L12" s="29"/>
+      <c r="L12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="L13" s="29"/>
+      <c r="L13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="L14" s="29"/>
+      <c r="L14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="L15" s="29"/>
+      <c r="L15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="L16" s="29"/>
+      <c r="L16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="30"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G19" s="28"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G20" s="28"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="28"/>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="28"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G25" s="28"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G26" s="30"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="25" t="s">
+      <c r="G28" s="31"/>
+      <c r="H28" s="26" t="s">
         <v>134</v>
       </c>
     </row>
@@ -12515,20 +12531,20 @@
       <c r="A29" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="25" t="s">
+      <c r="G29" s="31"/>
+      <c r="H29" s="26" t="s">
         <v>134</v>
       </c>
     </row>
@@ -12536,55 +12552,55 @@
       <c r="A30" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G30" s="30"/>
+      <c r="G30" s="31"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H32">

</xml_diff>